<commit_message>
incluir novo ficheiro agrupado da info serviços 2025
</commit_message>
<xml_diff>
--- a/DSD_2024_2025/ficheiros_servicos_ISA/2024_01_26 DSD_inform_202324_v6-1-1.xlsx (Dados MCaron e Carlos)_compact_ML3.xlsx
+++ b/DSD_2024_2025/ficheiros_servicos_ISA/2024_01_26 DSD_inform_202324_v6-1-1.xlsx (Dados MCaron e Carlos)_compact_ML3.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulisboa-my.sharepoint.com/personal/mlordel_office365_ulisboa_pt/Documents/Ambiente de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\cg-isa\DSD_2024_2025\ficheiros_servicos_ISA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="11_E30D009FD7797618CF5C73821380892E41B64493" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3AE7B68-B8B0-4065-9010-E147DF621299}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="planos_estudos" sheetId="1" r:id="rId1"/>
@@ -5292,7 +5291,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
@@ -5663,7 +5662,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y729"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -38471,14 +38470,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A464" workbookViewId="0">
-      <selection activeCell="G477" sqref="G477"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="100.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="74.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -57484,12 +57506,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -57808,7 +57837,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58404,7 +58433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58484,7 +58513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -58838,10 +58867,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H391"/>
   <sheetViews>
-    <sheetView topLeftCell="A374" workbookViewId="0">
+    <sheetView topLeftCell="A359" workbookViewId="0">
       <selection activeCell="C378" sqref="C378"/>
     </sheetView>
   </sheetViews>
@@ -66744,10 +66773,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -67049,10 +67078,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>